<commit_message>
updated the import file wih empty rows
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-with-some-empty-rows.xlsx
+++ b/tests/Data/Disks/Local/import-with-some-empty-rows.xlsx
@@ -1,42 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10907"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10907"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evidencemandizvidza/Sites/Laravel-Excel/tests/Data/Disks/Local/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evidencemandizvidza/Documents/Dukstra Technologies/File Uploads/Supplier Uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBD88E1-26AE-6C4B-8EDD-E6D056340872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900AF6FE-EDDD-0945-BAA1-40EDD479A292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{950D50D6-1905-420D-AFCC-60BF2AA9201C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+  <si>
+    <t>Test</t>
+  </si>
   <si>
     <t>test</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -59,14 +86,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -89,44 +120,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -154,14 +185,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -189,6 +237,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -200,206 +265,182 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B6C10D-4127-4A86-A16A-6996119904D0}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the import file with empty rows
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-with-some-empty-rows.xlsx
+++ b/tests/Data/Disks/Local/import-with-some-empty-rows.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evidencemandizvidza/Documents/Dukstra Technologies/File Uploads/Supplier Uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evidencemandizvidza/Sites/Laravel-Excel/tests/Data/Disks/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900AF6FE-EDDD-0945-BAA1-40EDD479A292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C4F39B-6C4E-B74B-B61A-4E2C31FD7F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{950D50D6-1905-420D-AFCC-60BF2AA9201C}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
-  <si>
-    <t>Test</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
   <si>
     <t>test</t>
   </si>
@@ -408,9 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B6C10D-4127-4A86-A16A-6996119904D0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -428,10 +423,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>